<commit_message>
Using CAPS for TOMES pattern syntax now.
</commit_message>
<xml_diff>
--- a/tests/sample_files/sampleEntityDictionary.xlsx
+++ b/tests/sample_files/sampleEntityDictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8100" windowWidth="20400" windowHeight="10410"/>
+    <workbookView xWindow="0" yWindow="8550" windowWidth="20400" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="3" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Should yield one manifestation with case-insensitive markup.</t>
   </si>
   <si>
-    <t>tomes_pattern: {"A","B"}, {"1","2"}</t>
-  </si>
-  <si>
     <t>Should yield 4 (2*2) manifestations.</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>Should ignore case sensitive instructions and yield 4 (2*2) manifestations.</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"A","B"}, {"1","2"}</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>9</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>9</v>
@@ -643,13 +643,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="1" t="b">
         <v>1</v>
@@ -663,13 +663,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="b">
         <v>0</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>

</xml_diff>